<commit_message>
- Created XlsxWriter class to allow saving data to xlsx files - Created CellDetails  model - Created Coordinate model
</commit_message>
<xml_diff>
--- a/src/template.xlsx
+++ b/src/template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\serku\Desktop\projects\python-excel\media\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\serku\Desktop\projects\python-excel\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Template</t>
   </si>
@@ -37,6 +37,15 @@
   </si>
   <si>
     <t>People per km</t>
+  </si>
+  <si>
+    <t>Today</t>
+  </si>
+  <si>
+    <t>Flag</t>
+  </si>
+  <si>
+    <t>Flag2</t>
   </si>
 </sst>
 </file>
@@ -117,7 +126,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -125,6 +134,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -405,10 +415,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -417,15 +427,18 @@
     <col min="2" max="2" width="14.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.28515625" style="3" customWidth="1"/>
     <col min="4" max="4" width="17.7109375" style="3" customWidth="1"/>
-    <col min="5" max="5" width="18.28515625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="18.140625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="19" style="3" customWidth="1"/>
+    <col min="7" max="7" width="23.140625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="24.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="21" customHeight="1">
+    <row r="1" spans="1:8" ht="21" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:8">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -441,20 +454,62 @@
       <c r="E2" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="F2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="3" spans="1:5">
-      <c r="C3" s="3">
+    <row r="3" spans="1:8">
+      <c r="C3">
         <v>5</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3">
         <v>4</v>
       </c>
       <c r="E3" s="4">
         <f>$C3/$D3</f>
         <v>1.25</v>
       </c>
+      <c r="F3" s="5">
+        <f ca="1">TODAY()</f>
+        <v>44233</v>
+      </c>
+      <c r="G3">
+        <f>MAX($C3:$D3)</f>
+        <v>5</v>
+      </c>
+      <c r="H3" s="3">
+        <f>MIN($C3:$D3)</f>
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="G3">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF7128"/>
+        <color rgb="FFFFEF9C"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H3">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF7128"/>
+        <color rgb="FFFFEF9C"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>